<commit_message>
second draft of tables.xlsx
</commit_message>
<xml_diff>
--- a/assets/tables.xlsx
+++ b/assets/tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SuperPotato\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RA\bondingcurves\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26FF1874-3888-408D-ABFF-83C03C62DF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB19F8F-9930-439E-97C4-1C6CA9347FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{78257B4B-863B-0240-9C5F-4DB116BF817F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{78257B4B-863B-0240-9C5F-4DB116BF817F}"/>
   </bookViews>
   <sheets>
     <sheet name="LitReview" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="103">
   <si>
     <t>DEX</t>
   </si>
@@ -230,18 +230,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> 3.6 million ether</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Synthetix hack: 37M sETH stolen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>bZx hack: $900k stolen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Oracle attack</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -254,10 +242,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>i</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>over $2 billion</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -286,22 +270,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>DAO \cite{Daian2016}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ethereum \cite{CryptoGroundTeam2020}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ethereum \cite{Shahda2019}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ethereum \cite{Bahrynovska2017}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Thodex \cite{Shaurya2021}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -339,10 +307,6 @@
   </si>
   <si>
     <t>56.98879 WETH = $237,569.16</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> $50m</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -448,6 +412,58 @@
       </rPr>
       <t>}</t>
     </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GovernMental \cite{Bahrynovska2017}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lendf.Me \cite{validnetwork2020}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$25m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bZx \cite{CryptoGroundTeam2020}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$900k stolen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Origin \cite{Khatri2020}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>7,137 ETH (worth about $3.3 million) and 2.25 million DAI (worth about $2.25 million).</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grim Finance \cite{Buchvarov2021}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$30m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtoZ Markets \cite{Mandzikasvili2019}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>37 million synthetic Ether (sETH)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integral \cite{Foxley2021}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>attracted $239 million</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -617,7 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -641,13 +657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -657,11 +667,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -677,6 +687,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -999,48 +1018,48 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="26.875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.84375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.15234375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.15234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.4609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.61328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.3828125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8.84375" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.3828125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.15234375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11" t="s">
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-    </row>
-    <row r="5" spans="3:17" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+    </row>
+    <row r="5" spans="3:17" s="5" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1087,7 +1106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:17" ht="31" x14ac:dyDescent="0.35">
       <c r="C6" s="8" t="s">
         <v>6</v>
       </c>
@@ -1134,7 +1153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1181,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:17" ht="31" x14ac:dyDescent="0.35">
       <c r="C8" s="8" t="s">
         <v>29</v>
       </c>
@@ -1228,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:17" ht="31" x14ac:dyDescent="0.35">
       <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
@@ -1275,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
@@ -1322,7 +1341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="3:17" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:17" ht="81" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C11" s="8" t="s">
         <v>22</v>
       </c>
@@ -1369,7 +1388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:17" ht="31" x14ac:dyDescent="0.35">
       <c r="C12" s="8" t="s">
         <v>24</v>
       </c>
@@ -1416,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:17" ht="31" x14ac:dyDescent="0.35">
       <c r="C13" s="8" t="s">
         <v>26</v>
       </c>
@@ -1463,7 +1482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="C14" s="8" t="s">
         <v>41</v>
       </c>
@@ -1510,7 +1529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:17" ht="31" x14ac:dyDescent="0.35">
       <c r="C15" s="8" t="s">
         <v>31</v>
       </c>
@@ -1557,7 +1576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:17" ht="31" x14ac:dyDescent="0.35">
       <c r="C16" s="8" t="s">
         <v>38</v>
       </c>
@@ -1604,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:17" ht="31" x14ac:dyDescent="0.35">
       <c r="C17" s="8" t="s">
         <v>33</v>
       </c>
@@ -1651,7 +1670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17" ht="31" x14ac:dyDescent="0.35">
       <c r="C18" s="9" t="s">
         <v>43</v>
       </c>
@@ -1712,316 +1731,317 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C3EE4C-B2C3-954E-B787-28F524DF8822}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F1" sqref="B1:F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11" style="12"/>
-    <col min="2" max="2" width="26.625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.125" customWidth="1"/>
-    <col min="4" max="4" width="49.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37" customWidth="1"/>
-    <col min="6" max="6" width="81.5" customWidth="1"/>
+    <col min="1" max="1" width="11" style="11"/>
+    <col min="2" max="2" width="24.84375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="96.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.07421875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="81.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B2" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="16"/>
+      <c r="C4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="16"/>
+      <c r="C5" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="16"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="16"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="16"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="15" t="s">
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="16"/>
+      <c r="C10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="16"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="16"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="16"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="16"/>
+      <c r="C15" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="16"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="16"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="124" x14ac:dyDescent="0.35">
+      <c r="B18" s="16"/>
+      <c r="C18" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="31" x14ac:dyDescent="0.35">
+      <c r="B19" s="16"/>
+      <c r="C19" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="16"/>
+      <c r="C20" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" s="15" t="s">
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="16"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="16"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="16"/>
+      <c r="C23" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="23"/>
+      <c r="E23" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="17" t="s">
+      <c r="F23" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="126" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>90</v>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="16"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B11:B21"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
+  <mergeCells count="14">
+    <mergeCell ref="D23:D24"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B24"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D20:D22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
third draft for tables
</commit_message>
<xml_diff>
--- a/assets/tables.xlsx
+++ b/assets/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RA\bondingcurves\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB19F8F-9930-439E-97C4-1C6CA9347FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FCAB4F-6195-43A3-BB90-F2D467EB8C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{78257B4B-863B-0240-9C5F-4DB116BF817F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{78257B4B-863B-0240-9C5F-4DB116BF817F}"/>
   </bookViews>
   <sheets>
     <sheet name="LitReview" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="136">
   <si>
     <t>DEX</t>
   </si>
@@ -191,131 +191,6 @@
   </si>
   <si>
     <t>Block timestamp manipulation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Transaction sequence manipulation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Other infrastructure-layer attacks</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Middleware-layer attacks</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reentrancy attack</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Other middleware-layer attacks</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Frontrunning</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Backrunning</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sandwich attacks</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1100 ETH jackpot payout was stuck with several reasons including timestamp manipulations</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Oracle attack</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>$100 million worth of loans were liquidated</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rug  pull</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>over $2 billion</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>$58 million</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>a loss of $280 million to unsuspecting traders each month worldwide</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vampire attack</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Harvest Finance \cite{Redman2020}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ethereum \cite{Redman2020}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compound \cite{Chong2020}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thodex \cite{Shaurya2021}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Uranium Finance \cite{Shaurya2021}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnubisDAO \cite{Shaurya2021}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>\cite{Mikalauskas2021}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>\cite{Dzyatkovskii2021}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wrapped Ether \cite{Alchemist2021}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SushiSwap \cite{Jakub2020}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>predators make around $4,000 daily on sandwiching globally</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>over $30 million</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>56.98879 WETH = $237,569.16</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gained $830 million</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>33MM USD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -323,20 +198,190 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="16"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Jiang2021, Davidson2020</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <t>GovernMental \cite{Bahrynovska2017}</t>
+  </si>
+  <si>
+    <t>1100 ETH jackpot payout was stuck with several reasons including timestamp manipulations</t>
+  </si>
+  <si>
+    <t>Transaction sequence manipulation</t>
+  </si>
+  <si>
+    <t>\cite{Han1996}</t>
+  </si>
+  <si>
+    <t>europarl.europa.eu cite\{Robby2018}</t>
+  </si>
+  <si>
+    <t>distributed denial-of-service (DDoS) attacks</t>
+  </si>
+  <si>
+    <t>\cit{Hui2017, Cheng2011, Rodrigues2019}</t>
+  </si>
+  <si>
+    <t>WEI Tech Exchange
+\cite{Greg LaBrie2018}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> loss of 119,756 coins. At the time of the break in, the loss was approximately $60 million. </t>
+  </si>
+  <si>
+    <t>blockchain denial-of-service (BDoS) attacks</t>
+  </si>
+  <si>
+    <t>\cit{Mirkin2020}</t>
+  </si>
+  <si>
+    <t>Bradley
+\cite{Law  2019}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 million bitcoin </t>
+  </si>
+  <si>
+    <t>network mining control attack</t>
+  </si>
+  <si>
+    <t>\cit{Zhou2021, Helmy2021, Eskandari2019}</t>
+  </si>
+  <si>
+    <t>Cointelegraph
+\cite{Mrie2019}</t>
+  </si>
+  <si>
+    <t>about 40k ETC</t>
+  </si>
+  <si>
+    <t>domain name server (DNS) hijacking</t>
+  </si>
+  <si>
+    <t>\cite{Dai2017, Patsakis2020, Aranjo2016}</t>
+  </si>
+  <si>
+    <t>CNN
+\cite{Josiah2017}</t>
+  </si>
+  <si>
+    <t>lost 17 percent of its assets</t>
+  </si>
+  <si>
+    <t>border gateway protocol (BGP) hijacking</t>
+  </si>
+  <si>
+    <t>\cite{Mastilak2020, MacDonald2009, Chakraborty2015}</t>
+  </si>
+  <si>
+    <t>The Cloudflare Blog
+\cite{Tom2019}</t>
+  </si>
+  <si>
+    <t>worst of the incident, of about 15% of our global traffic.</t>
+  </si>
+  <si>
+    <t>Middleware-layer attacks</t>
+  </si>
+  <si>
+    <t>Reentrancy attack</t>
+  </si>
+  <si>
+    <t>\cite{Fatima2020, Liu2018, Alkhalifah2021}</t>
+  </si>
+  <si>
+    <t>Lendf.Me \cite{validnetwork2020}</t>
+  </si>
+  <si>
+    <t>$25m</t>
+  </si>
+  <si>
+    <t>bZx \cite{CryptoGroundTeam2020}</t>
+  </si>
+  <si>
+    <t>$900k stolen</t>
+  </si>
+  <si>
+    <t>Origin \cite{Khatri2020}</t>
+  </si>
+  <si>
+    <t>7,137 ETH (worth about $3.3 million) and 2.25 million DAI (worth about $2.25 million).</t>
+  </si>
+  <si>
+    <t>Grim Finance \cite{Buchvarov2021}</t>
+  </si>
+  <si>
+    <t>$30m</t>
+  </si>
+  <si>
+    <t>middleware-layer attacks: 
+replay attack</t>
+  </si>
+  <si>
+    <t>\cite{khazraei2017, zhou2021, chiou2013}</t>
+  </si>
+  <si>
+    <t>coindesk
+\cite{Alyssa2016}</t>
+  </si>
+  <si>
+    <t>40,000 ETC</t>
+  </si>
+  <si>
+    <t>middleware-layer attacks:
+exception mishandling</t>
+  </si>
+  <si>
+    <t>\cite{luu2016, popescu2020, mense2018}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">middleware-layer attacks: integer under-flow/overflow attacks </t>
+  </si>
+  <si>
+    <t>\cite{Praitheesha2019, Moona2021}</t>
+  </si>
+  <si>
+    <t>Medium
+\cite{HaloBlock2018}</t>
+  </si>
+  <si>
+    <t>could cause a catastrophic loss for the crypto holder’s account</t>
+  </si>
+  <si>
+    <t>Oracle attack</t>
+  </si>
+  <si>
+    <r>
+      <t>\cite{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
         <color theme="1"/>
         <rFont val="Tahoma"/>
-        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t>﻿</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="16"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -344,38 +389,71 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="16"/>
         <color theme="1"/>
         <rFont val="Tahoma"/>
-        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t>﻿</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="16"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>gudgeon2020}</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>\cite{Fatima2020, Liu2018, Alkhalifah2021}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compound \cite{Chong2020}</t>
+  </si>
+  <si>
+    <t>$100 million worth of loans were liquidated</t>
+  </si>
+  <si>
+    <t>Ethereum \cite{Redman2020}</t>
+  </si>
+  <si>
+    <t>over $30 million</t>
+  </si>
+  <si>
+    <t>AtoZ Markets \cite{Mandzikasvili2019}</t>
+  </si>
+  <si>
+    <t>37 million synthetic Ether (sETH)</t>
+  </si>
+  <si>
+    <t>Harvest Finance \cite{Redman2020}</t>
+  </si>
+  <si>
+    <t>33MM USD</t>
+  </si>
+  <si>
+    <t>Rug  pull</t>
   </si>
   <si>
     <t>\cite{Xia2021}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>\cite{Zhou2021High-Frequency Trading on Decentralized On-Chain Exchanges, Angeris2021}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uranium Finance \cite{Shaurya2021}</t>
+  </si>
+  <si>
+    <t>Thodex \cite{Shaurya2021}</t>
+  </si>
+  <si>
+    <t>over $2 billion</t>
+  </si>
+  <si>
+    <t>AnubisDAO \cite{Shaurya2021}</t>
+  </si>
+  <si>
+    <t>$58 million</t>
+  </si>
+  <si>
+    <t>Frontrunning</t>
   </si>
   <si>
     <t>\cite{Zhou2021High-Frequency Trading on Decentralized On-Chain Exchanges, 
@@ -383,88 +461,61 @@
 Daian2019, 
 Angeris2021, 
 Zhou2021A2MM: Mitigating Frontrunning, Transaction Reordering and Consensus Instability in Decentralized Exchanges}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\cite{Mikalauskas2021}</t>
+  </si>
+  <si>
+    <t>a loss of $280 million to unsuspecting traders each month worldwide</t>
+  </si>
+  <si>
+    <t>Backrunning</t>
+  </si>
+  <si>
+    <t>\cite{Zhou2021High-Frequency Trading on Decentralized On-Chain Exchanges, Angeris2021}</t>
+  </si>
+  <si>
+    <t>Coindesk
+\cite{Daniel2020}</t>
+  </si>
+  <si>
+    <t>moved than 807,000 ETC</t>
+  </si>
+  <si>
+    <t>Sandwich attacks</t>
   </si>
   <si>
     <t>\cite{Züst2021, Dunkelman2010, Zhou2021High-Frequency Trading on Decentralized On-Chain Exchanges, }</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>\cite{</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Jiang2021, Davidson2020</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>}</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GovernMental \cite{Bahrynovska2017}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lendf.Me \cite{validnetwork2020}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>$25m</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>bZx \cite{CryptoGroundTeam2020}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>$900k stolen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Origin \cite{Khatri2020}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>7,137 ETH (worth about $3.3 million) and 2.25 million DAI (worth about $2.25 million).</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Grim Finance \cite{Buchvarov2021}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>$30m</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AtoZ Markets \cite{Mandzikasvili2019}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>37 million synthetic Ether (sETH)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\cite{Dzyatkovskii2021}</t>
+  </si>
+  <si>
+    <t>predators make around $4,000 daily on sandwiching globally</t>
+  </si>
+  <si>
+    <t>Wrapped Ether \cite{Alchemist2021}</t>
+  </si>
+  <si>
+    <t>56.98879 WETH = $237,569.16</t>
+  </si>
+  <si>
+    <t>Vampire attack</t>
+  </si>
+  <si>
+    <t>\cite{Lo2020, mr2016, gsssietwdetection}</t>
+  </si>
+  <si>
+    <t>SushiSwap \cite{Jakub2020}</t>
+  </si>
+  <si>
+    <t>gained $830 million</t>
   </si>
   <si>
     <t>Integral \cite{Foxley2021}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>attracted $239 million</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -503,32 +554,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="16"/>
       <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="16"/>
       <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -633,7 +680,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -658,44 +705,39 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1018,48 +1060,48 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="26.84375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.15234375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.15234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.4609375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.61328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.3828125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.3828125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8.875" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.375" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.15234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15" t="s">
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-    </row>
-    <row r="5" spans="3:17" s="5" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+    </row>
+    <row r="5" spans="3:17" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1106,7 +1148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C6" s="8" t="s">
         <v>6</v>
       </c>
@@ -1153,7 +1195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:17" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1200,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
         <v>29</v>
       </c>
@@ -1247,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
@@ -1294,7 +1336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:17" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
@@ -1341,7 +1383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="3:17" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:17" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="8" t="s">
         <v>22</v>
       </c>
@@ -1388,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="3:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="s">
         <v>24</v>
       </c>
@@ -1435,7 +1477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="3:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="s">
         <v>26</v>
       </c>
@@ -1482,7 +1524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="3:17" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C14" s="8" t="s">
         <v>41</v>
       </c>
@@ -1529,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C15" s="8" t="s">
         <v>31</v>
       </c>
@@ -1576,7 +1618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="3:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C16" s="8" t="s">
         <v>38</v>
       </c>
@@ -1623,7 +1665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C17" s="8" t="s">
         <v>33</v>
       </c>
@@ -1670,7 +1712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C18" s="9" t="s">
         <v>43</v>
       </c>
@@ -1731,317 +1773,418 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C3EE4C-B2C3-954E-B787-28F524DF8822}">
-  <dimension ref="A2:F24"/>
+  <dimension ref="A2:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F1" sqref="B1:F24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="11"/>
-    <col min="2" max="2" width="24.84375" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="96.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.07421875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="81.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.75" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="16" t="s">
+    <row r="3" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="13" t="s">
+      <c r="D3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="13"/>
+      <c r="C4" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="16"/>
-      <c r="C4" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="16"/>
-      <c r="C5" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="17" t="s">
+      <c r="F5" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="13"/>
+      <c r="C6" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
+      <c r="C8" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+      <c r="C9" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="13"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="16"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="16"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="16"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="16"/>
-      <c r="C10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="16"/>
+    </row>
+    <row r="12" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="13"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
-      <c r="E12" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="16"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="13" t="s">
+      <c r="E12" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="13"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="13"/>
+      <c r="C14" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
+      <c r="C15" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="2:6" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="13"/>
+      <c r="C16" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="F13" t="s">
+      <c r="D17" s="17" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="16"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="16"/>
-      <c r="C15" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="13" t="s">
+      <c r="E17" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="B19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="13"/>
+      <c r="C21" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="16"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="16"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="124" x14ac:dyDescent="0.35">
-      <c r="B18" s="16"/>
-      <c r="C18" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="31" x14ac:dyDescent="0.35">
-      <c r="B19" s="16"/>
-      <c r="C19" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="16"/>
-      <c r="C20" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="16"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="16"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="16"/>
-      <c r="C23" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="16"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>102</v>
+    <row r="22" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="243" x14ac:dyDescent="0.25">
+      <c r="B24" s="13"/>
+      <c r="C24" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="81" x14ac:dyDescent="0.25">
+      <c r="B25" s="13"/>
+      <c r="C25" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="13"/>
+      <c r="C26" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B27" s="13"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="13"/>
+      <c r="C28" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="13"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="B17:B29"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="B11:B24"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="B10:B16"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
4th draft for tables
</commit_message>
<xml_diff>
--- a/assets/tables.xlsx
+++ b/assets/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RA\bondingcurves\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FCAB4F-6195-43A3-BB90-F2D467EB8C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFEC2FA-AFD4-43BD-8CB5-751412ED1C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{78257B4B-863B-0240-9C5F-4DB116BF817F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{78257B4B-863B-0240-9C5F-4DB116BF817F}"/>
   </bookViews>
   <sheets>
     <sheet name="LitReview" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="121">
   <si>
     <t>DEX</t>
   </si>
@@ -200,6 +200,7 @@
       <rPr>
         <sz val="16"/>
         <rFont val="等线"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>Jiang2021, Davidson2020</t>
@@ -208,6 +209,7 @@
       <rPr>
         <sz val="16"/>
         <rFont val="等线"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -215,154 +217,217 @@
     </r>
   </si>
   <si>
-    <t>GovernMental \cite{Bahrynovska2017}</t>
-  </si>
-  <si>
-    <t>1100 ETH jackpot payout was stuck with several reasons including timestamp manipulations</t>
+    <t xml:space="preserve">4 million bitcoin </t>
+  </si>
+  <si>
+    <t>about 40k ETC</t>
+  </si>
+  <si>
+    <t>lost 17 percent of its assets</t>
+  </si>
+  <si>
+    <t>Middleware-layer attacks</t>
+  </si>
+  <si>
+    <t>Reentrancy attack</t>
+  </si>
+  <si>
+    <t>\cite{Fatima2020, Liu2018, Alkhalifah2021}</t>
+  </si>
+  <si>
+    <t>$25m</t>
+  </si>
+  <si>
+    <t>bZx \cite{CryptoGroundTeam2020}</t>
+  </si>
+  <si>
+    <t>$900k stolen</t>
+  </si>
+  <si>
+    <t>7,137 ETH (worth about $3.3 million) and 2.25 million DAI (worth about $2.25 million).</t>
+  </si>
+  <si>
+    <t>Grim Finance \cite{Buchvarov2021}</t>
+  </si>
+  <si>
+    <t>$30m</t>
+  </si>
+  <si>
+    <t>Oracle attack</t>
+  </si>
+  <si>
+    <t>Compound \cite{Chong2020}</t>
+  </si>
+  <si>
+    <t>$100 million worth of loans were liquidated</t>
+  </si>
+  <si>
+    <t>over $30 million</t>
+  </si>
+  <si>
+    <t>AtoZ Markets \cite{Mandzikasvili2019}</t>
+  </si>
+  <si>
+    <t>37 million synthetic Ether (sETH)</t>
+  </si>
+  <si>
+    <t>Harvest Finance \cite{Redman2020}</t>
+  </si>
+  <si>
+    <t>33MM USD</t>
+  </si>
+  <si>
+    <t>Rug  pull</t>
+  </si>
+  <si>
+    <t>over $2 billion</t>
+  </si>
+  <si>
+    <t>$58 million</t>
+  </si>
+  <si>
+    <t>Frontrunning</t>
+  </si>
+  <si>
+    <t>Backrunning</t>
+  </si>
+  <si>
+    <t>Sandwich attacks</t>
+  </si>
+  <si>
+    <t>Vampire attack</t>
+  </si>
+  <si>
+    <t>SushiSwap \cite{Jakub2020}</t>
+  </si>
+  <si>
+    <t>gained $830 million</t>
+  </si>
+  <si>
+    <t>attracted $239 million</t>
   </si>
   <si>
     <t>Transaction sequence manipulation</t>
-  </si>
-  <si>
-    <t>\cite{Han1996}</t>
-  </si>
-  <si>
-    <t>europarl.europa.eu cite\{Robby2018}</t>
-  </si>
-  <si>
-    <t>distributed denial-of-service (DDoS) attacks</t>
-  </si>
-  <si>
-    <t>\cit{Hui2017, Cheng2011, Rodrigues2019}</t>
-  </si>
-  <si>
-    <t>WEI Tech Exchange
-\cite{Greg LaBrie2018}</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> loss of 119,756 coins. At the time of the break in, the loss was approximately $60 million. </t>
-  </si>
-  <si>
-    <t>blockchain denial-of-service (BDoS) attacks</t>
-  </si>
-  <si>
-    <t>\cit{Mirkin2020}</t>
-  </si>
-  <si>
-    <t>Bradley
-\cite{Law  2019}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 million bitcoin </t>
-  </si>
-  <si>
-    <t>network mining control attack</t>
-  </si>
-  <si>
-    <t>\cit{Zhou2021, Helmy2021, Eskandari2019}</t>
-  </si>
-  <si>
-    <t>Cointelegraph
-\cite{Mrie2019}</t>
-  </si>
-  <si>
-    <t>about 40k ETC</t>
-  </si>
-  <si>
-    <t>domain name server (DNS) hijacking</t>
-  </si>
-  <si>
-    <t>\cite{Dai2017, Patsakis2020, Aranjo2016}</t>
-  </si>
-  <si>
-    <t>CNN
-\cite{Josiah2017}</t>
-  </si>
-  <si>
-    <t>lost 17 percent of its assets</t>
-  </si>
-  <si>
-    <t>border gateway protocol (BGP) hijacking</t>
-  </si>
-  <si>
-    <t>\cite{Mastilak2020, MacDonald2009, Chakraborty2015}</t>
-  </si>
-  <si>
-    <t>The Cloudflare Blog
-\cite{Tom2019}</t>
-  </si>
-  <si>
-    <t>worst of the incident, of about 15% of our global traffic.</t>
-  </si>
-  <si>
-    <t>Middleware-layer attacks</t>
-  </si>
-  <si>
-    <t>Reentrancy attack</t>
-  </si>
-  <si>
-    <t>\cite{Fatima2020, Liu2018, Alkhalifah2021}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\cite{Houben2018}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Distributed denial-of-service (DDoS) attacks</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\cite{Hui2017, Cheng2011, Rodrigues2019}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeversiFi \cite{Greg2018, Foltýn2017, Phillips2020}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bitfinex loss of 119,756 coins. At the time of the break in, the loss was approximately $60 million. DeversiFi, which spawned out of Bitfinex—was also affected by the attack.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blockchain denial-of-service (BDoS) attacks</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\cite{Mirkin2020}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BitGo \cite{Law3602019}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Network mining control attack</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\cite{Zhou2021A2MM, Helmy2021, Eskandari2020}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gate.io \cite{Huillet2019}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Domain name server (DNS) hijacking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\cite{Dai2017, Patsakis2020, Aranjo2019}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EtherDelta \cite{Wilmoth2017}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Border gateway protocol (BGP) hijacking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\cite{Mastilak2020, MacDonald2009, Chakraborty2015Security}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Lendf.Me \cite{validnetwork2020}</t>
-  </si>
-  <si>
-    <t>$25m</t>
-  </si>
-  <si>
-    <t>bZx \cite{CryptoGroundTeam2020}</t>
-  </si>
-  <si>
-    <t>$900k stolen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Origin \cite{Khatri2020}</t>
-  </si>
-  <si>
-    <t>7,137 ETH (worth about $3.3 million) and 2.25 million DAI (worth about $2.25 million).</t>
-  </si>
-  <si>
-    <t>Grim Finance \cite{Buchvarov2021}</t>
-  </si>
-  <si>
-    <t>$30m</t>
-  </si>
-  <si>
-    <t>middleware-layer attacks: 
-replay attack</t>
-  </si>
-  <si>
-    <t>\cite{khazraei2017, zhou2021, chiou2013}</t>
-  </si>
-  <si>
-    <t>coindesk
-\cite{Alyssa2016}</t>
-  </si>
-  <si>
-    <t>40,000 ETC</t>
-  </si>
-  <si>
-    <t>middleware-layer attacks:
-exception mishandling</t>
-  </si>
-  <si>
-    <t>\cite{luu2016, popescu2020, mense2018}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">middleware-layer attacks: integer under-flow/overflow attacks </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Replay attack</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>\cite{khazraei2017,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Zhou2021A2MM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Chiou2013}</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exception mishandling</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\cite{luu2016making, Popescu, Mense2018}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer under-flow/overflow attacks </t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>\cite{Praitheesha2019, Moona2021}</t>
-  </si>
-  <si>
-    <t>Medium
-\cite{HaloBlock2018}</t>
-  </si>
-  <si>
-    <t>could cause a catastrophic loss for the crypto holder’s account</t>
-  </si>
-  <si>
-    <t>Oracle attack</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -373,7 +438,7 @@
         <sz val="16"/>
         <color theme="1"/>
         <rFont val="Tahoma"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>﻿</t>
     </r>
@@ -382,6 +447,7 @@
         <sz val="16"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -392,7 +458,7 @@
         <sz val="16"/>
         <color theme="1"/>
         <rFont val="Tahoma"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>﻿</t>
     </r>
@@ -401,121 +467,61 @@
         <sz val="16"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>gudgeon2020}</t>
     </r>
-  </si>
-  <si>
-    <t>Compound \cite{Chong2020}</t>
-  </si>
-  <si>
-    <t>$100 million worth of loans were liquidated</t>
-  </si>
-  <si>
-    <t>Ethereum \cite{Redman2020}</t>
-  </si>
-  <si>
-    <t>over $30 million</t>
-  </si>
-  <si>
-    <t>AtoZ Markets \cite{Mandzikasvili2019}</t>
-  </si>
-  <si>
-    <t>37 million synthetic Ether (sETH)</t>
-  </si>
-  <si>
-    <t>Harvest Finance \cite{Redman2020}</t>
-  </si>
-  <si>
-    <t>33MM USD</t>
-  </si>
-  <si>
-    <t>Rug  pull</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Curve \cite{Redman2020}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>\cite{Xia2021}</t>
-  </si>
-  <si>
-    <t>Uranium Finance \cite{Shaurya2021}</t>
-  </si>
-  <si>
-    <t>Thodex \cite{Shaurya2021}</t>
-  </si>
-  <si>
-    <t>over $2 billion</t>
-  </si>
-  <si>
-    <t>AnubisDAO \cite{Shaurya2021}</t>
-  </si>
-  <si>
-    <t>$58 million</t>
-  </si>
-  <si>
-    <t>Frontrunning</t>
-  </si>
-  <si>
-    <t>\cite{Zhou2021High-Frequency Trading on Decentralized On-Chain Exchanges, 
-Eskandari2020, 
-Daian2019, 
-Angeris2021, 
-Zhou2021A2MM: Mitigating Frontrunning, Transaction Reordering and Consensus Instability in Decentralized Exchanges}</t>
-  </si>
-  <si>
-    <t>\cite{Mikalauskas2021}</t>
-  </si>
-  <si>
-    <t>a loss of $280 million to unsuspecting traders each month worldwide</t>
-  </si>
-  <si>
-    <t>Backrunning</t>
-  </si>
-  <si>
-    <t>\cite{Zhou2021High-Frequency Trading on Decentralized On-Chain Exchanges, Angeris2021}</t>
-  </si>
-  <si>
-    <t>Coindesk
-\cite{Daniel2020}</t>
-  </si>
-  <si>
-    <t>moved than 807,000 ETC</t>
-  </si>
-  <si>
-    <t>Sandwich attacks</t>
-  </si>
-  <si>
-    <t>\cite{Züst2021, Dunkelman2010, Zhou2021High-Frequency Trading on Decentralized On-Chain Exchanges, }</t>
-  </si>
-  <si>
-    <t>\cite{Dzyatkovskii2021}</t>
-  </si>
-  <si>
-    <t>predators make around $4,000 daily on sandwiching globally</t>
-  </si>
-  <si>
-    <t>Wrapped Ether \cite{Alchemist2021}</t>
-  </si>
-  <si>
-    <t>56.98879 WETH = $237,569.16</t>
-  </si>
-  <si>
-    <t>Vampire attack</t>
-  </si>
-  <si>
-    <t>\cite{Lo2020, mr2016, gsssietwdetection}</t>
-  </si>
-  <si>
-    <t>SushiSwap \cite{Jakub2020}</t>
-  </si>
-  <si>
-    <t>gained $830 million</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uranium Finance \cite{Malwa2021}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thodex \cite{Malwa2021}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnubisDAO \cite{Malwa2021}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\cite{Zhou2021High-Frequency, Eskandari2020, Daian2019, Angeris2021, Zhou2021A2MM}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a loss of $280 million to unsuspecting traders each month worldwide \cite{Mikalauskas2021}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\cite{Zhou2021High-Frequency, Angeris2021}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\cite{Züst2021, Dunkelman2010, Zhou2021High-Frequency}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>predators make around $4,000 daily on sandwiching globally \cite{Dzyatkovskii2021}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\cite{Lo2020UniswapExchange, Dangare2016}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Integral \cite{Foxley2021}</t>
-  </si>
-  <si>
-    <t>attracted $239 million</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -557,25 +563,28 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -586,7 +595,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -623,64 +632,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -708,36 +665,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1773,418 +1741,379 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C3EE4C-B2C3-954E-B787-28F524DF8822}">
-  <dimension ref="A2:F29"/>
+  <dimension ref="A2:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="11"/>
-    <col min="2" max="2" width="34.75" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="64.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="126" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="127" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B4" s="13"/>
-      <c r="C4" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="15"/>
+      <c r="C4" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B6" s="13"/>
+      <c r="C6" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
+      <c r="C8" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B9" s="20"/>
+      <c r="C9" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="E10" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="15" t="s">
+    </row>
+    <row r="11" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
-      <c r="C6" s="15" t="s">
+    <row r="12" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B12" s="13"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="15" t="s">
+    </row>
+    <row r="13" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B13" s="13"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="F13" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="15" t="s">
+    </row>
+    <row r="14" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B14" s="13"/>
+      <c r="C14" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
+      <c r="C15" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B16" s="13"/>
+      <c r="C16" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="25" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="15" t="s">
+      <c r="D17" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="F17" s="23" t="s">
         <v>67</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
-      <c r="C9" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="13"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="13"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
-      <c r="C15" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-    </row>
-    <row r="16" spans="2:6" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B19" s="13"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B20" s="13"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B21" s="13"/>
       <c r="C21" s="17" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="15" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="15" t="s">
-        <v>113</v>
+      <c r="F22" s="14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B23" s="13"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="15" t="s">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B24" s="13"/>
+      <c r="C24" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="E24" s="14"/>
+      <c r="F24" s="14" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="243" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="15" t="s">
+    <row r="25" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B25" s="13"/>
+      <c r="C25" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B26" s="13"/>
+      <c r="C26" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E26" s="14"/>
+      <c r="F26" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="81" x14ac:dyDescent="0.25">
-      <c r="B25" s="13"/>
-      <c r="C25" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
-      <c r="C26" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B27" s="13"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>129</v>
+      <c r="C27" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="13"/>
-      <c r="C28" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="13"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>135</v>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="12">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="B10:B16"/>
+    <mergeCell ref="B17:B28"/>
+    <mergeCell ref="C27:C28"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="D10:D13"/>
-    <mergeCell ref="B17:B29"/>
     <mergeCell ref="C17:C20"/>
     <mergeCell ref="D17:D20"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="D21:D23"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="B10:B16"/>
+    <mergeCell ref="D27:D28"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add a nee table tab
</commit_message>
<xml_diff>
--- a/assets/tables.xlsx
+++ b/assets/tables.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RA\bondingcurves\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiahuaxu/GitHub/bondingcurves/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFEC2FA-AFD4-43BD-8CB5-751412ED1C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109F1790-9AE1-BD48-A1EA-27C24E640817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{78257B4B-863B-0240-9C5F-4DB116BF817F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{78257B4B-863B-0240-9C5F-4DB116BF817F}"/>
   </bookViews>
   <sheets>
     <sheet name="LitReview" sheetId="1" r:id="rId1"/>
     <sheet name="attacks" sheetId="2" r:id="rId2"/>
+    <sheet name="AMMprotocols" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,8 +35,71 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={F266C8A2-D118-284E-B6FC-DBB4CE6BEEA2}</author>
+    <author>tc={8FEFD333-10DF-E743-9752-CFC05D11E325}</author>
+    <author>tc={645C4158-2567-DD4B-A149-A2DC276E67F5}</author>
+    <author>tc={3BFD043E-7E3B-3249-A7C3-EEBA99361266}</author>
+    <author>tc={2F7C9FDE-CAD7-3945-A0AE-E7E45033B1F1}</author>
+    <author>tc={7C07A7B0-6E52-4F43-909D-826D6D2BF894}</author>
+  </authors>
+  <commentList>
+    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{F266C8A2-D118-284E-B6FC-DBB4CE6BEEA2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is actually a way to protect LPs, so is 'part of' the next column</t>
+      </text>
+    </comment>
+    <comment ref="J10" authorId="1" shapeId="0" xr:uid="{8FEFD333-10DF-E743-9752-CFC05D11E325}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not sure</t>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="2" shapeId="0" xr:uid="{645C4158-2567-DD4B-A149-A2DC276E67F5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not sure</t>
+      </text>
+    </comment>
+    <comment ref="J11" authorId="3" shapeId="0" xr:uid="{3BFD043E-7E3B-3249-A7C3-EEBA99361266}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not sure</t>
+      </text>
+    </comment>
+    <comment ref="M11" authorId="4" shapeId="0" xr:uid="{2F7C9FDE-CAD7-3945-A0AE-E7E45033B1F1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not sure</t>
+      </text>
+    </comment>
+    <comment ref="R14" authorId="5" shapeId="0" xr:uid="{7C07A7B0-6E52-4F43-909D-826D6D2BF894}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Can look at date of contract creation https://etherscan.io/tx/0x750f6632f7884defd40b79be8174bbb44de9ef21ca4172a249d7a4fe10b45e8e</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="204">
   <si>
     <t>DEX</t>
   </si>
@@ -208,7 +272,7 @@
     <r>
       <rPr>
         <sz val="16"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -393,7 +457,7 @@
     <r>
       <rPr>
         <sz val="16"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -404,7 +468,7 @@
       <rPr>
         <sz val="16"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -446,7 +510,7 @@
       <rPr>
         <sz val="16"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -466,7 +530,7 @@
       <rPr>
         <sz val="16"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -523,16 +587,265 @@
     <t>Integral \cite{Foxley2021}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Ethereum</t>
+  </si>
+  <si>
+    <t>Financial derivative</t>
+  </si>
+  <si>
+    <t>APWine</t>
+  </si>
+  <si>
+    <t>Prediction market</t>
+  </si>
+  <si>
+    <t>Augur</t>
+  </si>
+  <si>
+    <t>EulerBeats</t>
+  </si>
+  <si>
+    <t>UMA</t>
+  </si>
+  <si>
+    <t>Pods Finance</t>
+  </si>
+  <si>
+    <t>Stablecoin</t>
+  </si>
+  <si>
+    <t>GyroScope</t>
+  </si>
+  <si>
+    <t>Gnosis</t>
+  </si>
+  <si>
+    <t>Yield space</t>
+  </si>
+  <si>
+    <t>Notional finance</t>
+  </si>
+  <si>
+    <t>DeFi embedded with AMM</t>
+  </si>
+  <si>
+    <t>QuipuSwap</t>
+  </si>
+  <si>
+    <t>Tezos</t>
+  </si>
+  <si>
+    <t>dynamic swap fee</t>
+  </si>
+  <si>
+    <t>multi-asset</t>
+  </si>
+  <si>
+    <t>Pure AMM</t>
+  </si>
+  <si>
+    <t>Kyber2021whitepaper</t>
+  </si>
+  <si>
+    <t>Kyber 3.0</t>
+  </si>
+  <si>
+    <t>asset-pair</t>
+  </si>
+  <si>
+    <t>Andersson2020</t>
+  </si>
+  <si>
+    <t>mStable</t>
+  </si>
+  <si>
+    <t>mooniswap2020whitepaper</t>
+  </si>
+  <si>
+    <t>Mooniswap</t>
+  </si>
+  <si>
+    <t>Polkadot</t>
+  </si>
+  <si>
+    <t>HydraDX</t>
+  </si>
+  <si>
+    <t>Not live</t>
+  </si>
+  <si>
+    <t>Tron</t>
+  </si>
+  <si>
+    <t>TrueSwap</t>
+  </si>
+  <si>
+    <t>Solana</t>
+  </si>
+  <si>
+    <t>StableSwap</t>
+  </si>
+  <si>
+    <t>Vampire Attack on Uniswap v2 (dale2020sushiswapvampire)</t>
+  </si>
+  <si>
+    <t>sushi2020</t>
+  </si>
+  <si>
+    <t>SushiSwap</t>
+  </si>
+  <si>
+    <t>Ethereum, EOS</t>
+  </si>
+  <si>
+    <t>divergence loss insurance</t>
+  </si>
+  <si>
+    <t>Bancor2020</t>
+  </si>
+  <si>
+    <t>Bancor V2.1</t>
+  </si>
+  <si>
+    <t>Bancor V2</t>
+  </si>
+  <si>
+    <t>https://etherscan.io/tx/0x750f6632f7884defd40b79be8174bbb44de9ef21ca4172a249d7a4fe10b45e8e</t>
+  </si>
+  <si>
+    <t>Hertzog2018</t>
+  </si>
+  <si>
+    <t>Bancor V1</t>
+  </si>
+  <si>
+    <t>Ethereum, BSC</t>
+  </si>
+  <si>
+    <t>single-asset</t>
+  </si>
+  <si>
+    <t>dodo2020whitepaper</t>
+  </si>
+  <si>
+    <t>DODO</t>
+  </si>
+  <si>
+    <t>Harvest Attack (cao2021flashot), Value.Defi Attack (cao2021flashot)</t>
+  </si>
+  <si>
+    <t>Egorov2019</t>
+  </si>
+  <si>
+    <t>Curve</t>
+  </si>
+  <si>
+    <t>Balancer V2</t>
+  </si>
+  <si>
+    <t>Balancer Attack (1inch2020balancerAttack)</t>
+  </si>
+  <si>
+    <t>martinelli2019whitepaper</t>
+  </si>
+  <si>
+    <t>Balancer V1</t>
+  </si>
+  <si>
+    <t>adams2021v3core</t>
+  </si>
+  <si>
+    <t>Uniswap V3</t>
+  </si>
+  <si>
+    <t>Harvest Attack (cao2021flashot), Cheesebank Attack (cao2021flashot), Value.Defi Attack (cao2021flashot), Warp Finance Attack  (cao2021flashot)</t>
+  </si>
+  <si>
+    <t>Core2020</t>
+  </si>
+  <si>
+    <t>Uniswap V2</t>
+  </si>
+  <si>
+    <t>bZx Oracle Attack (cao2021flashot)</t>
+  </si>
+  <si>
+    <t>Adams2018</t>
+  </si>
+  <si>
+    <t>Uniswap V1</t>
+  </si>
+  <si>
+    <t>miannet launch</t>
+  </si>
+  <si>
+    <t>Chain</t>
+  </si>
+  <si>
+    <t>Front-running</t>
+  </si>
+  <si>
+    <t>liquidity provider protection</t>
+  </si>
+  <si>
+    <t>divergenve loss compensation</t>
+  </si>
+  <si>
+    <t>time decay</t>
+  </si>
+  <si>
+    <t>capital concentration</t>
+  </si>
+  <si>
+    <t>oracle price component</t>
+  </si>
+  <si>
+    <t>constant-product component</t>
+  </si>
+  <si>
+    <t>constant-sum component</t>
+  </si>
+  <si>
+    <t>pool structure</t>
+  </si>
+  <si>
+    <t>Protocol application</t>
+  </si>
+  <si>
+    <t>cite</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Associated attacks</t>
+  </si>
+  <si>
+    <t>AMM add-on features</t>
+  </si>
+  <si>
+    <t>conservation function components</t>
+  </si>
+  <si>
+    <t>insurance</t>
+  </si>
+  <si>
+    <t>\mathcal{A}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -540,13 +853,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -555,21 +868,21 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -586,13 +899,44 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -637,7 +981,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -662,12 +1006,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -677,20 +1015,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -701,18 +1027,526 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="17" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -725,8 +1559,41 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Xu, Jiahua" id="{036DB0A5-9A37-1742-A3F7-59B74AD43F60}" userId="S::ucacjxu@ucl.ac.uk::7a6344da-4ad5-4eee-bc02-f3951f0e55d7" providerId="AD"/>
+  <person displayName="simon.cousaert" id="{1AE7033E-D555-3941-9328-6407986EA49C}" userId="S::simon.cousaert_outlook.com#ext#@liveuclac.onmicrosoft.com::3509a644-7812-48a3-9060-60422aa578e3" providerId="AD"/>
+</personList>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4654A54-1774-274F-8193-5337C1C82680}" name="Table1" displayName="Table1" ref="B5:R34" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="B5:R34" xr:uid="{008D2199-0F15-2F4F-A092-430F9EAE67BD}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{7DD0AFA2-3DC3-7A40-8883-D17ED974E011}" name="Name" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{5A0E83A9-E6F4-5E41-B7C7-1702542DC3BF}" name="cite" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{A48EA57B-872C-0A4C-B462-4CBBD75B8F26}" name="Protocol application" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{5E73C893-7054-8A4C-9040-09D83072307F}" name="pool structure" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{7D009CD3-5D78-4748-80BA-2EA2F38E309A}" name="constant-sum component" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{16DFB123-F0A1-B945-91D1-888A04AB30F1}" name="constant-product component" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{F30DC0B4-43D5-B44C-B530-B058ED92CD29}" name="oracle price component" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{B05FB6D0-D14D-0546-99CE-1E93CAFB4606}" name="capital concentration" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{B4C7EAF4-DA52-AD4C-B999-3BE5766272ED}" name="time decay" dataDxfId="10"/>
+    <tableColumn id="17" xr3:uid="{EC6E61C9-A980-7A4C-9EA6-3E774C296BFE}" name="divergenve loss compensation" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{88AC795C-9D6D-CF43-8328-5C1F0576795C}" name="dynamic swap fee" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{A8B1B674-1AAC-E648-AFD5-07F354189A33}" name="liquidity provider protection" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{485B62E1-248A-1245-A71C-01A2CF6D0D11}" name="Oracle attack" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{D180EB55-80FA-1D46-A3D1-0125A6DE89C4}" name="Vampire attack" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{303058AD-6354-D64F-9947-CD6296FA1F66}" name="Front-running" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{D18029F6-74CF-7F40-9938-A6D349A14C24}" name="Chain" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{F3CCBA67-7803-C24D-B01B-7491DD2CF112}" name="miannet launch" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1020,6 +1887,29 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="L5" dT="2021-04-13T13:56:53.59" personId="{1AE7033E-D555-3941-9328-6407986EA49C}" id="{F266C8A2-D118-284E-B6FC-DBB4CE6BEEA2}">
+    <text>This is actually a way to protect LPs, so is 'part of' the next column</text>
+  </threadedComment>
+  <threadedComment ref="J10" dT="2021-04-13T12:39:36.33" personId="{1AE7033E-D555-3941-9328-6407986EA49C}" id="{8FEFD333-10DF-E743-9752-CFC05D11E325}">
+    <text>Not sure</text>
+  </threadedComment>
+  <threadedComment ref="M10" dT="2021-04-13T12:39:27.83" personId="{1AE7033E-D555-3941-9328-6407986EA49C}" id="{645C4158-2567-DD4B-A149-A2DC276E67F5}">
+    <text>Not sure</text>
+  </threadedComment>
+  <threadedComment ref="J11" dT="2021-04-13T12:39:36.33" personId="{1AE7033E-D555-3941-9328-6407986EA49C}" id="{3BFD043E-7E3B-3249-A7C3-EEBA99361266}">
+    <text>Not sure</text>
+  </threadedComment>
+  <threadedComment ref="M11" dT="2021-04-13T12:39:27.83" personId="{1AE7033E-D555-3941-9328-6407986EA49C}" id="{2F7C9FDE-CAD7-3945-A0AE-E7E45033B1F1}">
+    <text>Not sure</text>
+  </threadedComment>
+  <threadedComment ref="R14" dT="2021-04-13T16:50:49.16" personId="{036DB0A5-9A37-1742-A3F7-59B74AD43F60}" id="{7C07A7B0-6E52-4F43-909D-826D6D2BF894}">
+    <text>Can look at date of contract creation https://etherscan.io/tx/0x750f6632f7884defd40b79be8174bbb44de9ef21ca4172a249d7a4fe10b45e8e</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1736A125-551E-9245-AA4F-F348FEC249A4}">
   <dimension ref="C4:Q18"/>
@@ -1028,48 +1918,48 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="26.875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" s="1" customFormat="1">
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12" t="s">
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12" t="s">
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-    </row>
-    <row r="5" spans="3:17" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+    </row>
+    <row r="5" spans="3:17" s="5" customFormat="1" ht="34">
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1116,7 +2006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:17" ht="34">
       <c r="C6" s="8" t="s">
         <v>6</v>
       </c>
@@ -1163,7 +2053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:17" ht="51">
       <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1210,7 +2100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:17" ht="34">
       <c r="C8" s="8" t="s">
         <v>29</v>
       </c>
@@ -1257,7 +2147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:17" ht="34">
       <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
@@ -1304,7 +2194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:17" ht="51">
       <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
@@ -1351,7 +2241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="3:17" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:17" ht="81" customHeight="1">
       <c r="C11" s="8" t="s">
         <v>22</v>
       </c>
@@ -1398,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:17" ht="34">
       <c r="C12" s="8" t="s">
         <v>24</v>
       </c>
@@ -1445,7 +2335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:17" ht="51">
       <c r="C13" s="8" t="s">
         <v>26</v>
       </c>
@@ -1492,7 +2382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:17" ht="51">
       <c r="C14" s="8" t="s">
         <v>41</v>
       </c>
@@ -1539,7 +2429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:17" ht="34">
       <c r="C15" s="8" t="s">
         <v>31</v>
       </c>
@@ -1586,7 +2476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:17" ht="34">
       <c r="C16" s="8" t="s">
         <v>38</v>
       </c>
@@ -1633,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:17" ht="34">
       <c r="C17" s="8" t="s">
         <v>33</v>
       </c>
@@ -1680,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17" ht="34">
       <c r="C18" s="9" t="s">
         <v>43</v>
       </c>
@@ -1743,380 +2633,1718 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C3EE4C-B2C3-954E-B787-28F524DF8822}">
   <dimension ref="A2:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11" style="11"/>
     <col min="2" max="2" width="38.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="126" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="127" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="2:6" ht="22">
+      <c r="B2" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="19" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+    <row r="3" spans="2:6" ht="22">
+      <c r="B3" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-    </row>
-    <row r="4" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B4" s="13"/>
-      <c r="C4" s="14" t="s">
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="2:6" ht="22">
+      <c r="B4" s="22"/>
+      <c r="C4" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="13"/>
-      <c r="C5" s="14" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="2:6" ht="44">
+      <c r="B5" s="22"/>
+      <c r="C5" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
-      <c r="C6" s="14" t="s">
+    <row r="6" spans="2:6" ht="22">
+      <c r="B6" s="22"/>
+      <c r="C6" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="14" t="s">
+    <row r="7" spans="2:6" ht="22">
+      <c r="B7" s="22"/>
+      <c r="C7" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="14" t="s">
+    <row r="8" spans="2:6" ht="22">
+      <c r="B8" s="22"/>
+      <c r="C8" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
-      <c r="C9" s="22" t="s">
+    <row r="9" spans="2:6" ht="22">
+      <c r="B9" s="23"/>
+      <c r="C9" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="2:6" ht="22">
+      <c r="B10" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="14" t="s">
+    <row r="11" spans="2:6" ht="22">
+      <c r="B11" s="22"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="13"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="14" t="s">
+    <row r="12" spans="2:6" ht="22">
+      <c r="B12" s="22"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="13"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="14" t="s">
+    <row r="13" spans="2:6" ht="22">
+      <c r="B13" s="22"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="14" t="s">
+    <row r="14" spans="2:6" ht="22">
+      <c r="B14" s="22"/>
+      <c r="C14" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
-      <c r="C15" s="14" t="s">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="2:6" ht="22">
+      <c r="B15" s="22"/>
+      <c r="C15" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="14" t="s">
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="2:6" ht="22">
+      <c r="B16" s="22"/>
+      <c r="C16" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="2:6" ht="22">
+      <c r="B17" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="17" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="14" t="s">
+    <row r="18" spans="2:6" ht="22">
+      <c r="B18" s="22"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="12" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B19" s="13"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="14" t="s">
+    <row r="19" spans="2:6" ht="22">
+      <c r="B19" s="22"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="14" t="s">
+    <row r="20" spans="2:6" ht="22">
+      <c r="B20" s="22"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="13"/>
-      <c r="C21" s="17" t="s">
+    <row r="21" spans="2:6" ht="22">
+      <c r="B21" s="22"/>
+      <c r="C21" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B22" s="13"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="14" t="s">
+    <row r="22" spans="2:6" ht="22">
+      <c r="B22" s="22"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="13"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="14" t="s">
+    <row r="23" spans="2:6" ht="22">
+      <c r="B23" s="22"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="14" t="s">
+    <row r="24" spans="2:6" ht="22">
+      <c r="B24" s="22"/>
+      <c r="C24" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14" t="s">
+      <c r="E24" s="12"/>
+      <c r="F24" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B25" s="13"/>
-      <c r="C25" s="14" t="s">
+    <row r="25" spans="2:6" ht="22">
+      <c r="B25" s="22"/>
+      <c r="C25" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-    </row>
-    <row r="26" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
-      <c r="C26" s="14" t="s">
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="2:6" ht="22">
+      <c r="B26" s="22"/>
+      <c r="C26" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14" t="s">
+      <c r="E26" s="12"/>
+      <c r="F26" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B27" s="13"/>
-      <c r="C27" s="17" t="s">
+    <row r="27" spans="2:6" ht="22">
+      <c r="B27" s="22"/>
+      <c r="C27" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="22" t="s">
+    <row r="28" spans="2:6" ht="22">
+      <c r="B28" s="23"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="16" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="D21:D23"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="B10:B16"/>
     <mergeCell ref="B17:B28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="D27:D28"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE940E80-B413-2F4C-AA8E-FE20B0E7100E}">
+  <dimension ref="A1:T34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.83203125" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" customWidth="1"/>
+    <col min="13" max="13" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.6640625" customWidth="1"/>
+    <col min="15" max="17" width="26.5" customWidth="1"/>
+    <col min="18" max="18" width="16.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:20">
+      <c r="E1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="2:20">
+      <c r="E2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" t="s">
+        <v>203</v>
+      </c>
+      <c r="M2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20">
+      <c r="E3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20">
+      <c r="F4" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+    </row>
+    <row r="5" spans="2:20">
+      <c r="B5" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="K5" t="s">
+        <v>189</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q5" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="R5" s="28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20">
+      <c r="B6" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R6" s="28"/>
+    </row>
+    <row r="7" spans="2:20" ht="17">
+      <c r="B7" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L7" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R7" s="31">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" ht="85">
+      <c r="B8" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L8" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R8" s="31">
+        <v>43952</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" ht="34">
+      <c r="B9" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L9" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R9" s="31">
+        <v>44317</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" ht="34">
+      <c r="B10" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L10" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R10" s="31">
+        <v>43891</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" ht="17">
+      <c r="B11" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L11" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R11" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" ht="51">
+      <c r="B12" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L12" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R12" s="31">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" ht="34">
+      <c r="B13" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="R13" s="31">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" ht="17">
+      <c r="B14" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E14" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="R14" s="31">
+        <v>42896</v>
+      </c>
+      <c r="T14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" ht="17">
+      <c r="B15" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" t="s">
+        <v>143</v>
+      </c>
+      <c r="F15" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L15" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="R15" s="31">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" ht="17">
+      <c r="B16" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E16" t="s">
+        <v>143</v>
+      </c>
+      <c r="F16" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>159</v>
+      </c>
+      <c r="L16" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="R16" s="31">
+        <v>44105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="34">
+      <c r="B17" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" t="s">
+        <v>143</v>
+      </c>
+      <c r="F17" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L17" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M17" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" s="28"/>
+      <c r="O17" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R17" s="31">
+        <v>44044</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="17">
+      <c r="A18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E18" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L18" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M18" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="R18" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="17">
+      <c r="A19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" t="s">
+        <v>143</v>
+      </c>
+      <c r="F19" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L19" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M19" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="R19" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="17">
+      <c r="A20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E20" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L20" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M20" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="R20" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="34">
+      <c r="B21" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F21" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L21" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M21" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R21" s="31">
+        <v>44044</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="34">
+      <c r="B22" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E22" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L22" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M22" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R22" s="31">
+        <v>44013</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="34">
+      <c r="B23" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E23" t="s">
+        <v>139</v>
+      </c>
+      <c r="F23" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>138</v>
+      </c>
+      <c r="L23" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="28"/>
+      <c r="Q23" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="R23" s="28"/>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="B24" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="B25" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="28"/>
+      <c r="Q25" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R25" s="28"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="B26" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R26" s="28"/>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="B27" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="28"/>
+      <c r="Q27" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R27" s="28"/>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="B28" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R28" s="28"/>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="B29" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R29" s="28"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="B30" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R30" s="28"/>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="B31" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="28"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="28"/>
+      <c r="Q31" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R31" s="28"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="B32" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R32" s="28"/>
+    </row>
+    <row r="33" spans="2:18">
+      <c r="B33" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="28"/>
+      <c r="Q33" s="28"/>
+      <c r="R33" s="28"/>
+    </row>
+    <row r="34" spans="2:18">
+      <c r="B34" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="R34" s="27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="O9:R9 M6:Q6 F6:L7 M7:R8 M9 N18:R18 M10:R17 K25:K34 F19:J34 L19:R34 F8:J17 L8:L17 K17:K22 K8:K15">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{339F8281-92ED-9E41-9F4A-9D5FC20D1765}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:J18 L18:M18">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C0E631E8-6425-034D-856C-909CD002EDC7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{339F8281-92ED-9E41-9F4A-9D5FC20D1765}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>O9:R9 M6:Q6 F6:L7 M7:R8 M9 N18:R18 M10:R17 K25:K34 F19:J34 L19:R34 F8:J17 L8:L17 K17:K22 K8:K15</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C0E631E8-6425-034D-856C-909CD002EDC7}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F18:J18 L18:M18</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>